<commit_message>
Updated Cell names and centered figure titles
</commit_message>
<xml_diff>
--- a/STA Outlines/STA Cell Outline Names.xlsx
+++ b/STA Outlines/STA Cell Outline Names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.sfwmd.gov\dfsroot\data\rsd_sta\STA_vegetation\STA_Vegetation_monitoring\SAV Surveys\R Script for Map and Figure Creation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d612b085ce925e02/Desktop/SAV-Survey-Figures/STA Outlines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04777398-8490-4F51-8D07-9173B54A206D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{04777398-8490-4F51-8D07-9173B54A206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCDB152C-0734-4B55-9483-1E181D88BC80}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{48D7FE87-0ABA-4D31-B615-F0E9B6B19885}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48D7FE87-0ABA-4D31-B615-F0E9B6B19885}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -204,88 +204,88 @@
     <t>CELL NAMES</t>
   </si>
   <si>
-    <t>STA-1E C4N</t>
-  </si>
-  <si>
-    <t>STA-1E C4S</t>
-  </si>
-  <si>
-    <t>STA-1E C6</t>
-  </si>
-  <si>
-    <t>STA-1W C1A</t>
-  </si>
-  <si>
-    <t>STA-1W C1B</t>
-  </si>
-  <si>
-    <t>STA-1W C2A</t>
-  </si>
-  <si>
-    <t>STA-1W C2B</t>
-  </si>
-  <si>
-    <t>STA-1W C3</t>
-  </si>
-  <si>
-    <t>STA-1W C4</t>
-  </si>
-  <si>
-    <t>STA-1W C5A</t>
-  </si>
-  <si>
-    <t>STA-1W C5B</t>
-  </si>
-  <si>
-    <t>STA-2 C2</t>
-  </si>
-  <si>
-    <t>STA-2 C3</t>
-  </si>
-  <si>
-    <t>STA-2 C4</t>
-  </si>
-  <si>
-    <t>STA-2 C5</t>
-  </si>
-  <si>
-    <t>STA-2 C6</t>
-  </si>
-  <si>
-    <t>STA-2 C8</t>
-  </si>
-  <si>
-    <t>STA-34 C1B</t>
-  </si>
-  <si>
-    <t>STA-34 C2B</t>
-  </si>
-  <si>
-    <t>STA-34 C3B</t>
-  </si>
-  <si>
-    <t>STA-56 C1A</t>
-  </si>
-  <si>
-    <t>STA-56 C1B</t>
-  </si>
-  <si>
-    <t>STA-56 C2A</t>
-  </si>
-  <si>
-    <t>STA-56 C2B</t>
-  </si>
-  <si>
-    <t>STA-56 C3A</t>
-  </si>
-  <si>
-    <t>STA-56 C3B</t>
-  </si>
-  <si>
-    <t>STA-56 C4B</t>
-  </si>
-  <si>
-    <t>STA-56 C5B</t>
+    <t>STA-1E Cell 4N</t>
+  </si>
+  <si>
+    <t>STA-1E Cell 4S</t>
+  </si>
+  <si>
+    <t>STA-1E Cell 6</t>
+  </si>
+  <si>
+    <t>STA-1W Cell 1A</t>
+  </si>
+  <si>
+    <t>STA-1W Cell 1B</t>
+  </si>
+  <si>
+    <t>STA-1W Cell 2A</t>
+  </si>
+  <si>
+    <t>STA-1W Cell 2B</t>
+  </si>
+  <si>
+    <t>STA-1W Cell 3</t>
+  </si>
+  <si>
+    <t>STA-1W Cell 4</t>
+  </si>
+  <si>
+    <t>STA-1W Cell 5A</t>
+  </si>
+  <si>
+    <t>STA-1W Cell 5B</t>
+  </si>
+  <si>
+    <t>STA-2 Cell 2</t>
+  </si>
+  <si>
+    <t>STA-2 Cell 3</t>
+  </si>
+  <si>
+    <t>STA-2 Cell 4</t>
+  </si>
+  <si>
+    <t>STA-2 Cell 5</t>
+  </si>
+  <si>
+    <t>STA-2 Cell 6</t>
+  </si>
+  <si>
+    <t>STA-2 Cell 8</t>
+  </si>
+  <si>
+    <t>STA-34 Cell 1B</t>
+  </si>
+  <si>
+    <t>STA-34 Cell 2B</t>
+  </si>
+  <si>
+    <t>STA-34 Cell 3B</t>
+  </si>
+  <si>
+    <t>STA-56 Cell 1A</t>
+  </si>
+  <si>
+    <t>STA-56 Cell 1B</t>
+  </si>
+  <si>
+    <t>STA-56 Cell 2A</t>
+  </si>
+  <si>
+    <t>STA-56 Cell 2B</t>
+  </si>
+  <si>
+    <t>STA-56 Cell 3A</t>
+  </si>
+  <si>
+    <t>STA-56 Cell 3B</t>
+  </si>
+  <si>
+    <t>STA-56 Cell 4B</t>
+  </si>
+  <si>
+    <t>STA-56 Cell 5B</t>
   </si>
 </sst>
 </file>
@@ -932,12 +932,13 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C29"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fixed date format issue
</commit_message>
<xml_diff>
--- a/STA Outlines/STA Cell Outline Names.xlsx
+++ b/STA Outlines/STA Cell Outline Names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d612b085ce925e02/Desktop/SAV-Survey-Figures/STA Outlines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{04777398-8490-4F51-8D07-9173B54A206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCDB152C-0734-4B55-9483-1E181D88BC80}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{75F30413-A49D-49F3-AC71-A9D38237FDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{977B43F3-12FA-4033-AD3D-4FB5C1AE37C9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48D7FE87-0ABA-4D31-B615-F0E9B6B19885}"/>
+    <workbookView xWindow="58560" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{48D7FE87-0ABA-4D31-B615-F0E9B6B19885}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>REGION</t>
   </si>
@@ -204,95 +204,122 @@
     <t>CELL NAMES</t>
   </si>
   <si>
-    <t>STA-1E Cell 4N</t>
-  </si>
-  <si>
-    <t>STA-1E Cell 4S</t>
-  </si>
-  <si>
-    <t>STA-1E Cell 6</t>
-  </si>
-  <si>
-    <t>STA-1W Cell 1A</t>
-  </si>
-  <si>
-    <t>STA-1W Cell 1B</t>
-  </si>
-  <si>
-    <t>STA-1W Cell 2A</t>
-  </si>
-  <si>
-    <t>STA-1W Cell 2B</t>
-  </si>
-  <si>
-    <t>STA-1W Cell 3</t>
-  </si>
-  <si>
-    <t>STA-1W Cell 4</t>
-  </si>
-  <si>
-    <t>STA-1W Cell 5A</t>
-  </si>
-  <si>
-    <t>STA-1W Cell 5B</t>
-  </si>
-  <si>
-    <t>STA-2 Cell 2</t>
-  </si>
-  <si>
-    <t>STA-2 Cell 3</t>
-  </si>
-  <si>
-    <t>STA-2 Cell 4</t>
-  </si>
-  <si>
-    <t>STA-2 Cell 5</t>
-  </si>
-  <si>
-    <t>STA-2 Cell 6</t>
-  </si>
-  <si>
-    <t>STA-2 Cell 8</t>
-  </si>
-  <si>
-    <t>STA-34 Cell 1B</t>
-  </si>
-  <si>
-    <t>STA-34 Cell 2B</t>
-  </si>
-  <si>
-    <t>STA-34 Cell 3B</t>
-  </si>
-  <si>
-    <t>STA-56 Cell 1A</t>
-  </si>
-  <si>
-    <t>STA-56 Cell 1B</t>
-  </si>
-  <si>
-    <t>STA-56 Cell 2A</t>
-  </si>
-  <si>
-    <t>STA-56 Cell 2B</t>
-  </si>
-  <si>
-    <t>STA-56 Cell 3A</t>
-  </si>
-  <si>
-    <t>STA-56 Cell 3B</t>
-  </si>
-  <si>
-    <t>STA-56 Cell 4B</t>
-  </si>
-  <si>
-    <t>STA-56 Cell 5B</t>
+    <t>STA-1E C4N</t>
+  </si>
+  <si>
+    <t>STA-1E C4S</t>
+  </si>
+  <si>
+    <t>STA-1E C6</t>
+  </si>
+  <si>
+    <t>STA-1W C1A</t>
+  </si>
+  <si>
+    <t>STA-1W C1B</t>
+  </si>
+  <si>
+    <t>STA-1W C2A</t>
+  </si>
+  <si>
+    <t>STA-1W C2B</t>
+  </si>
+  <si>
+    <t>STA-1W C3</t>
+  </si>
+  <si>
+    <t>STA-1W C4</t>
+  </si>
+  <si>
+    <t>STA-1W C5A</t>
+  </si>
+  <si>
+    <t>STA-1W C5B</t>
+  </si>
+  <si>
+    <t>STA-2 C2</t>
+  </si>
+  <si>
+    <t>STA-2 C3</t>
+  </si>
+  <si>
+    <t>STA-2 C4</t>
+  </si>
+  <si>
+    <t>STA-2 C5</t>
+  </si>
+  <si>
+    <t>STA-2 C6</t>
+  </si>
+  <si>
+    <t>STA-2 C8</t>
+  </si>
+  <si>
+    <t>STA-34 C1B</t>
+  </si>
+  <si>
+    <t>STA-34 C2B</t>
+  </si>
+  <si>
+    <t>STA-34 C3B</t>
+  </si>
+  <si>
+    <t>STA-56 C1A</t>
+  </si>
+  <si>
+    <t>STA-56 C1B</t>
+  </si>
+  <si>
+    <t>STA-56 C2A</t>
+  </si>
+  <si>
+    <t>STA-56 C2B</t>
+  </si>
+  <si>
+    <t>STA-56 C3A</t>
+  </si>
+  <si>
+    <t>STA-56 C3B</t>
+  </si>
+  <si>
+    <t>STA-56 C4B</t>
+  </si>
+  <si>
+    <t>STA-56 C5B</t>
+  </si>
+  <si>
+    <t>STA1W_6</t>
+  </si>
+  <si>
+    <t>STA-1W C6</t>
+  </si>
+  <si>
+    <t>STA1W_7</t>
+  </si>
+  <si>
+    <t>STA-1W C7</t>
+  </si>
+  <si>
+    <t>STA1W_8</t>
+  </si>
+  <si>
+    <t>STA-1W C8</t>
+  </si>
+  <si>
+    <t>STA1W_6_11</t>
+  </si>
+  <si>
+    <t>STA1W_7_11</t>
+  </si>
+  <si>
+    <t>STA1W_8_11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +352,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -410,15 +443,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -622,8 +655,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3B9753C7-621B-4669-AB80-A8D2AD59D10C}" name="Table3" displayName="Table3" ref="A1:B29" totalsRowShown="0" tableBorderDxfId="2">
-  <autoFilter ref="A1:B29" xr:uid="{83399499-51C2-4D39-9280-4B9213A6EB41}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3B9753C7-621B-4669-AB80-A8D2AD59D10C}" name="Table3" displayName="Table3" ref="A1:B32" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="A1:B32" xr:uid="{83399499-51C2-4D39-9280-4B9213A6EB41}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F538A61F-A67A-42AF-9785-86C6B2750F89}" name="REGION" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{CC058E4F-8AA4-4B4F-82E0-42E0B9B2A565}" name="GIS outline" dataDxfId="0"/>
@@ -633,9 +666,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -673,7 +706,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -779,7 +812,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -921,7 +954,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -929,16 +962,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19486598-0751-4F46-97AC-56E84C6983C2}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1075,192 +1107,226 @@
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>87</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>89</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>91</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>